<commit_message>
Measured T and P units converted
</commit_message>
<xml_diff>
--- a/Data_proj2.xlsx
+++ b/Data_proj2.xlsx
@@ -1,14 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jc/Documents/classes/ME140/ME140Proj2/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17560" tabRatio="500" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Title" sheetId="1" r:id="rId3"/>
-    <sheet state="visible" name="CollectedData" sheetId="2" r:id="rId4"/>
-    <sheet state="visible" name="FlowAreas" sheetId="3" r:id="rId5"/>
+    <sheet name="Title" sheetId="1" r:id="rId1"/>
+    <sheet name="CollectedData" sheetId="2" r:id="rId2"/>
+    <sheet name="FlowAreas" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -102,120 +118,382 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="14" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="3">
-        <v>43201.0</v>
+        <v>43201</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:M11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -240,7 +518,7 @@
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2"/>
       <c r="B2" s="1" t="s">
         <v>11</v>
@@ -279,7 +557,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -320,19 +598,348 @@
         <v>27</v>
       </c>
     </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -341,6 +948,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>